<commit_message>
xls2xml - testando configuracao brisanet com container
</commit_message>
<xml_diff>
--- a/xls2xml/tests_box/input_json_brisanet_filme_teste_20210201.xlsx
+++ b/xls2xml/tests_box/input_json_brisanet_filme_teste_20210201.xlsx
@@ -398,7 +398,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="&quot;VERDADEIRO&quot;;&quot;VERDADEIRO&quot;;&quot;FALSO&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -577,7 +577,7 @@
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.33"/>
@@ -885,7 +885,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -904,7 +904,10 @@
       <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.64"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1533,7 +1536,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1552,11 +1555,11 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>